<commit_message>
Plantillas para resultados RCM
</commit_message>
<xml_diff>
--- a/Formulario para RCM.xlsx
+++ b/Formulario para RCM.xlsx
@@ -12,12 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4320" tabRatio="679" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos Evaluador" sheetId="9" r:id="rId1"/>
-    <sheet name="Formulario 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Formulario 2" sheetId="6" r:id="rId3"/>
-    <sheet name="Formulario 3" sheetId="7" r:id="rId4"/>
-    <sheet name="Formulario 4" sheetId="8" r:id="rId5"/>
-    <sheet name="datos" sheetId="11" state="hidden" r:id="rId6"/>
+    <sheet name="Formulario 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Formulario 2" sheetId="6" r:id="rId2"/>
+    <sheet name="Formulario 3" sheetId="7" r:id="rId3"/>
+    <sheet name="Formulario 4" sheetId="8" r:id="rId4"/>
+    <sheet name="datos" sheetId="11" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>Tipo de problema</t>
   </si>
@@ -152,12 +151,6 @@
   </si>
   <si>
     <t>Formulario RCM #1</t>
-  </si>
-  <si>
-    <t>Nombre de Evaluador</t>
-  </si>
-  <si>
-    <t>Nombre del Prototipo o Interfaz a Evaluar</t>
   </si>
   <si>
     <t>Si</t>
@@ -299,18 +292,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="14">
@@ -466,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -495,8 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -512,6 +497,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -547,12 +538,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1066,55 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+      <selection activeCell="C7" sqref="C7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,39 +1111,39 @@
       <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1220,41 +1160,41 @@
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1271,43 +1211,43 @@
       <c r="B15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,34 +1273,34 @@
       <c r="B21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1578,14 +1518,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="A3:G3"/>
@@ -1602,13 +1534,21 @@
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -1683,14 +1623,14 @@
       <c r="B5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1698,14 +1638,14 @@
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
       <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1723,14 +1663,14 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1738,69 +1678,69 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2117,11 +2057,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:J3"/>
     </sheetView>
   </sheetViews>
@@ -2192,14 +2132,14 @@
       <c r="B5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2207,14 +2147,14 @@
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
       <c r="K6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2232,14 +2172,14 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -2247,69 +2187,69 @@
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2627,12 +2567,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:F10"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2689,59 +2629,59 @@
       <c r="B5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2785,68 +2725,68 @@
       <c r="B15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3121,12 +3061,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C19:F19"/>
@@ -3136,13 +3070,19 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H9"/>
   <sheetViews>
@@ -3157,130 +3097,130 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
       <c r="F2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
-        <v>43</v>
+      <c r="B3" s="21" t="s">
+        <v>41</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>44</v>
+      <c r="D3" s="21" t="s">
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>45</v>
+      <c r="B4" s="21" t="s">
+        <v>43</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>46</v>
+      <c r="D4" s="21" t="s">
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="24" t="s">
-        <v>62</v>
+      <c r="H4" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>47</v>
+      <c r="B5" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>48</v>
+      <c r="D5" s="21" t="s">
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>63</v>
+      <c r="H5" s="22" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>49</v>
+      <c r="B6" s="21" t="s">
+        <v>47</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>50</v>
+      <c r="D6" s="21" t="s">
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="24" t="s">
-        <v>64</v>
+      <c r="H6" s="22" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>51</v>
+      <c r="B7" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>52</v>
+      <c r="D7" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="22" t="s">
-        <v>65</v>
+      <c r="H7" s="20" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>67</v>
+      <c r="H9" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>